<commit_message>
reorganized the whole backtesting code. separated methods in classes, depending on if its reliant on a particular strategy or not
</commit_message>
<xml_diff>
--- a/eeuuAnalysis/worldAnalysis.xlsx
+++ b/eeuuAnalysis/worldAnalysis.xlsx
@@ -462,13 +462,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>1.132155574745006</v>
+        <v>1.15</v>
       </c>
       <c r="C2" t="n">
-        <v>0.7684130982597326</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="D2" t="n">
-        <v>70.51917711128033</v>
+        <v>69.66</v>
       </c>
     </row>
     <row r="3">
@@ -478,13 +478,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.8741814676080708</v>
+        <v>0.88</v>
       </c>
       <c r="C3" t="n">
-        <v>-0.7966175551979429</v>
+        <v>-0.78</v>
       </c>
       <c r="D3" t="n">
-        <v>34.49673609568758</v>
+        <v>35.03</v>
       </c>
     </row>
     <row r="4">
@@ -494,13 +494,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1.019263530168315</v>
+        <v>1.03</v>
       </c>
       <c r="C4" t="n">
-        <v>0.09605518143031819</v>
+        <v>0.35</v>
       </c>
       <c r="D4" t="n">
-        <v>56.33630158238832</v>
+        <v>61.08</v>
       </c>
     </row>
     <row r="5">
@@ -510,13 +510,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.6619555490733783</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="C5" t="n">
-        <v>-1.42971675849289</v>
+        <v>-1.33</v>
       </c>
       <c r="D5" t="n">
-        <v>38.82823024659147</v>
+        <v>39.46</v>
       </c>
     </row>
     <row r="6">
@@ -526,13 +526,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.9370778437943629</v>
+        <v>0.9</v>
       </c>
       <c r="C6" t="n">
-        <v>-0.3560300624059426</v>
+        <v>-0.54</v>
       </c>
       <c r="D6" t="n">
-        <v>51.54507165030229</v>
+        <v>48.47</v>
       </c>
     </row>
     <row r="7">
@@ -542,13 +542,13 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.9062003530130208</v>
+        <v>0.91</v>
       </c>
       <c r="C7" t="n">
-        <v>-0.734747164714071</v>
+        <v>-0.68</v>
       </c>
       <c r="D7" t="n">
-        <v>36.98575861724121</v>
+        <v>38.04</v>
       </c>
     </row>
   </sheetData>

</xml_diff>